<commit_message>
chore: adding cost data
</commit_message>
<xml_diff>
--- a/model_costs.xlsx
+++ b/model_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dropbox\AI Projects\deer-age-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F50BEDA-6B94-47E7-A47C-0133311FC15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E143978-DC90-4E1F-B0EA-E0B3B2BA23DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="1740" windowWidth="14625" windowHeight="11295" xr2:uid="{FF094E04-538D-42CA-820E-B170657C60B9}"/>
   </bookViews>
@@ -316,6 +316,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -323,15 +332,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,7 +672,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,21 +686,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="I1" s="19" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="I1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="21"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -716,16 +716,16 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="23" t="s">
+      <c r="J2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -766,10 +766,18 @@
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="16"/>
+      <c r="I4" s="17">
+        <v>45884</v>
+      </c>
+      <c r="J4" s="5">
+        <v>9.48</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="L4" s="16">
+        <v>8.75</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>

</xml_diff>